<commit_message>
Auto update: 2025-11-27 21:30:26
</commit_message>
<xml_diff>
--- a/DECISION/미장_비트코인_분석.xlsx
+++ b/DECISION/미장_비트코인_분석.xlsx
@@ -492,19 +492,19 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>91727.27</v>
+        <v>91410.83</v>
       </c>
       <c r="E2">
-        <v>35.8</v>
+        <v>35</v>
       </c>
       <c r="F2">
-        <v>8.359999999999999</v>
+        <v>7.99</v>
       </c>
       <c r="G2">
         <v>30</v>
       </c>
       <c r="H2">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I2">
         <v>53</v>

</xml_diff>

<commit_message>
Auto update: 2025-11-28 00:20:55
</commit_message>
<xml_diff>
--- a/DECISION/미장_비트코인_분석.xlsx
+++ b/DECISION/미장_비트코인_분석.xlsx
@@ -49,7 +49,7 @@
     <t>판단</t>
   </si>
   <si>
-    <t>2025-11-27</t>
+    <t>2025-11-28</t>
   </si>
   <si>
     <t>Bitcoin USD</t>
@@ -492,13 +492,13 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>91410.83</v>
+        <v>90801.8</v>
       </c>
       <c r="E2">
-        <v>35</v>
+        <v>33.6</v>
       </c>
       <c r="F2">
-        <v>7.99</v>
+        <v>7.27</v>
       </c>
       <c r="G2">
         <v>30</v>
@@ -510,7 +510,7 @@
         <v>53</v>
       </c>
       <c r="J2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Auto update: 2025-12-01 01:14:42
</commit_message>
<xml_diff>
--- a/DECISION/미장_비트코인_분석.xlsx
+++ b/DECISION/미장_비트코인_분석.xlsx
@@ -572,13 +572,13 @@
         <v>22</v>
       </c>
       <c r="D3">
-        <v>91492.55</v>
+        <v>91475.77</v>
       </c>
       <c r="E3">
         <v>43.5</v>
       </c>
       <c r="F3">
-        <v>4.75</v>
+        <v>4.73</v>
       </c>
       <c r="G3">
         <v>40</v>

</xml_diff>